<commit_message>
Added < coords.txt argument to gdallocationinfo command. Reads values from all station in one call. Astropy did not work, replaced with pysolar. Added day_night function to select day/night observations masking night/day rows with NaN.
</commit_message>
<xml_diff>
--- a/Cor-Factor/Reg/results.xlsx
+++ b/Cor-Factor/Reg/results.xlsx
@@ -468,34 +468,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1.495751177961281</v>
+        <v>0.007307977243890207</v>
       </c>
       <c r="D2">
-        <v>0.01890327946828316</v>
+        <v>0.2042482159442283</v>
       </c>
       <c r="E2">
-        <v>0.4915788332939111</v>
+        <v>4.734106030302786</v>
       </c>
       <c r="F2">
-        <v>1.348611505733193e-236</v>
+        <v>1.737961192307855e-05</v>
       </c>
       <c r="G2">
-        <v>0.002439693617599025</v>
+        <v>0.9987761858899808</v>
       </c>
       <c r="H2">
-        <v>0.8129267847420415</v>
+        <v>0.380665828052104</v>
       </c>
       <c r="I2">
-        <v>2.699033036991987</v>
+        <v>5.825676796000084</v>
       </c>
       <c r="J2">
-        <v>5.697540822348791e-15</v>
+        <v>1.516402179975824e-15</v>
       </c>
       <c r="K2">
-        <v>646</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -503,34 +503,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="C3">
-        <v>0.4841953233579446</v>
+        <v>0.1550479081649281</v>
       </c>
       <c r="D3">
-        <v>0.02390227682525474</v>
+        <v>0.1161157312238916</v>
       </c>
       <c r="E3">
-        <v>0.6110677192850571</v>
+        <v>2.504872879457793</v>
       </c>
       <c r="F3">
-        <v>2.604533228064803e-182</v>
+        <v>2.336198482367304e-09</v>
       </c>
       <c r="G3">
-        <v>0.4284460872327484</v>
+        <v>0.9510833923457575</v>
       </c>
       <c r="H3">
-        <v>0.7393694991148736</v>
+        <v>0.7259421860880491</v>
       </c>
       <c r="I3">
-        <v>3.03203037921743</v>
+        <v>3.058852846571612</v>
       </c>
       <c r="J3">
-        <v>-1.652958868327212e-15</v>
+        <v>4.736951571734001e-15</v>
       </c>
       <c r="K3">
-        <v>619</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -541,31 +541,31 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="C4">
-        <v>1.007833721340485</v>
+        <v>7.548961188007898</v>
       </c>
       <c r="D4">
-        <v>0.0281710639006405</v>
+        <v>0.155068947513865</v>
       </c>
       <c r="E4">
-        <v>0.7583828456060212</v>
+        <v>3.58098173330632</v>
       </c>
       <c r="F4">
-        <v>1.847794974986693e-153</v>
+        <v>1.554158763801489e-07</v>
       </c>
       <c r="G4">
-        <v>0.1843456436985647</v>
+        <v>0.0418586844402117</v>
       </c>
       <c r="H4">
-        <v>0.6628208619246087</v>
+        <v>0.529180045017565</v>
       </c>
       <c r="I4">
-        <v>3.452284117740038</v>
+        <v>2.754992322690183</v>
       </c>
       <c r="J4">
-        <v>1.891833847000454e-14</v>
+        <v>-5.192427684400732e-15</v>
       </c>
       <c r="K4">
-        <v>643</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -573,34 +573,34 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1.52493650392173</v>
+        <v>3.991571880794022</v>
       </c>
       <c r="D5">
-        <v>0.0273653734356233</v>
+        <v>0.146500487672622</v>
       </c>
       <c r="E5">
-        <v>0.766835679327238</v>
+        <v>3.47558585552411</v>
       </c>
       <c r="F5">
-        <v>1.35386068652141e-149</v>
+        <v>2.045380335021598e-07</v>
       </c>
       <c r="G5">
-        <v>0.04723677334828091</v>
+        <v>0.2604958087660011</v>
       </c>
       <c r="H5">
-        <v>0.7071527624684776</v>
+        <v>0.6246302966024428</v>
       </c>
       <c r="I5">
-        <v>2.767606092563589</v>
+        <v>3.217232981367922</v>
       </c>
       <c r="J5">
-        <v>-4.711346428103007e-15</v>
+        <v>-1.474376176702208e-14</v>
       </c>
       <c r="K5">
-        <v>555</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -611,31 +611,31 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>3.1584348491646</v>
+        <v>6.380809795566059</v>
       </c>
       <c r="D6">
-        <v>0.03017369790224106</v>
+        <v>0.1435430695320799</v>
       </c>
       <c r="E6">
-        <v>0.8125518344303484</v>
+        <v>3.265438079660177</v>
       </c>
       <c r="F6">
-        <v>7.532705086060088e-134</v>
+        <v>1.418164207188511e-07</v>
       </c>
       <c r="G6">
-        <v>0.0001136899469721105</v>
+        <v>0.06075071653480218</v>
       </c>
       <c r="H6">
-        <v>0.6635163841569942</v>
+        <v>0.6341438957377079</v>
       </c>
       <c r="I6">
-        <v>2.742639677731559</v>
+        <v>2.909453587146678</v>
       </c>
       <c r="J6">
-        <v>5.084384513489089e-17</v>
+        <v>-1.01844458792281e-14</v>
       </c>
       <c r="K6">
-        <v>559</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -646,31 +646,31 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2.124322432199756</v>
+        <v>3.567888816915884</v>
       </c>
       <c r="D7">
-        <v>0.02663422763173771</v>
+        <v>0.1433839153537295</v>
       </c>
       <c r="E7">
-        <v>0.6960663284944156</v>
+        <v>3.366916192389526</v>
       </c>
       <c r="F7">
-        <v>6.555327667047998e-162</v>
+        <v>4.123936309411831e-08</v>
       </c>
       <c r="G7">
-        <v>0.002371106125943982</v>
+        <v>0.2965439946159347</v>
       </c>
       <c r="H7">
-        <v>0.694190740561929</v>
+        <v>0.5815430501635944</v>
       </c>
       <c r="I7">
-        <v>3.161293796224874</v>
+        <v>3.786860095324411</v>
       </c>
       <c r="J7">
-        <v>1.1678904677662e-14</v>
+        <v>2.592520792638203e-15</v>
       </c>
       <c r="K7">
-        <v>623</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -678,34 +678,34 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0.4917220907544895</v>
+        <v>0.02884030168999363</v>
       </c>
       <c r="D8">
-        <v>0.02458797165596778</v>
+        <v>0.1965765756382262</v>
       </c>
       <c r="E8">
-        <v>0.6262864138364225</v>
+        <v>4.585481204082646</v>
       </c>
       <c r="F8">
-        <v>2.123718328558734e-158</v>
+        <v>1.673343332618078e-05</v>
       </c>
       <c r="G8">
-        <v>0.4327552413057746</v>
+        <v>0.9950220535642406</v>
       </c>
       <c r="H8">
-        <v>0.7732662376420423</v>
+        <v>0.4549770928067196</v>
       </c>
       <c r="I8">
-        <v>2.986925950630678</v>
+        <v>5.221496034255939</v>
       </c>
       <c r="J8">
-        <v>-8.345594350200767e-15</v>
+        <v>7.105427357601002e-15</v>
       </c>
       <c r="K8">
-        <v>487</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -713,34 +713,34 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.3264607174840171</v>
+        <v>5.086357067735555</v>
       </c>
       <c r="D9">
-        <v>0.03425971966407697</v>
+        <v>0.06930718222530308</v>
       </c>
       <c r="E9">
-        <v>0.8719611697426995</v>
+        <v>1.480981933674747</v>
       </c>
       <c r="F9">
-        <v>9.833875709675654e-120</v>
+        <v>9.108925829895073e-15</v>
       </c>
       <c r="G9">
-        <v>0.7082320747627133</v>
+        <v>0.0018102221604539</v>
       </c>
       <c r="H9">
-        <v>0.5710415127903949</v>
+        <v>0.8777311088258974</v>
       </c>
       <c r="I9">
-        <v>4.76244329903263</v>
+        <v>1.723169989892944</v>
       </c>
       <c r="J9">
-        <v>-2.833316827953047e-15</v>
+        <v>-1.260640337638887e-14</v>
       </c>
       <c r="K9">
-        <v>642</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed pandas FutureWarning for matplotlib
Removed __init__ function from Modis, so that load_dataset() call is the same with Hobo.
</commit_message>
<xml_diff>
--- a/Cor-Factor/Reg/results.xlsx
+++ b/Cor-Factor/Reg/results.xlsx
@@ -468,34 +468,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="C2">
-        <v>0.007307977243890207</v>
+        <v>0.5674682166313563</v>
       </c>
       <c r="D2">
-        <v>0.2042482159442283</v>
+        <v>0.01178039961164318</v>
       </c>
       <c r="E2">
-        <v>4.734106030302786</v>
+        <v>0.2657729160057531</v>
       </c>
       <c r="F2">
-        <v>1.737961192307855e-05</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.9987761858899808</v>
+        <v>0.0329825307187054</v>
       </c>
       <c r="H2">
-        <v>0.380665828052104</v>
+        <v>0.874617094785566</v>
       </c>
       <c r="I2">
-        <v>5.825676796000084</v>
+        <v>2.934568162247113</v>
       </c>
       <c r="J2">
-        <v>1.516402179975824e-15</v>
+        <v>-1.84123248049139e-14</v>
       </c>
       <c r="K2">
-        <v>41</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -503,34 +503,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.1550479081649281</v>
+        <v>0.3070023891072907</v>
       </c>
       <c r="D3">
-        <v>0.1161157312238916</v>
+        <v>0.01407066102916952</v>
       </c>
       <c r="E3">
-        <v>2.504872879457793</v>
+        <v>0.31323995125622</v>
       </c>
       <c r="F3">
-        <v>2.336198482367304e-09</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.9510833923457575</v>
+        <v>0.3272735674166306</v>
       </c>
       <c r="H3">
-        <v>0.7259421860880491</v>
+        <v>0.8307545166893964</v>
       </c>
       <c r="I3">
-        <v>3.058852846571612</v>
+        <v>3.162758929044037</v>
       </c>
       <c r="J3">
-        <v>4.736951571734001e-15</v>
+        <v>3.115085514680555e-15</v>
       </c>
       <c r="K3">
-        <v>30</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -538,34 +538,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.9999999999999999</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="C4">
-        <v>7.548961188007898</v>
+        <v>0.2883889200526189</v>
       </c>
       <c r="D4">
-        <v>0.155068947513865</v>
+        <v>0.0166682876273685</v>
       </c>
       <c r="E4">
-        <v>3.58098173330632</v>
+        <v>0.3902297037166906</v>
       </c>
       <c r="F4">
-        <v>1.554158763801489e-07</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.0418586844402117</v>
+        <v>0.460060290463257</v>
       </c>
       <c r="H4">
-        <v>0.529180045017565</v>
+        <v>0.7766652926778326</v>
       </c>
       <c r="I4">
-        <v>2.754992322690183</v>
+        <v>3.937364482533346</v>
       </c>
       <c r="J4">
-        <v>-5.192427684400732e-15</v>
+        <v>5.728194089637838e-15</v>
       </c>
       <c r="K4">
-        <v>39</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -576,31 +576,31 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>3.991571880794022</v>
+        <v>0.4148163217381614</v>
       </c>
       <c r="D5">
-        <v>0.146500487672622</v>
+        <v>0.01343996622811544</v>
       </c>
       <c r="E5">
-        <v>3.47558585552411</v>
+        <v>0.3303914504409028</v>
       </c>
       <c r="F5">
-        <v>2.045380335021598e-07</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.2604958087660011</v>
+        <v>0.2095568041017632</v>
       </c>
       <c r="H5">
-        <v>0.6246302966024428</v>
+        <v>0.8361298594968598</v>
       </c>
       <c r="I5">
-        <v>3.217232981367922</v>
+        <v>3.165847911001365</v>
       </c>
       <c r="J5">
-        <v>-1.474376176702208e-14</v>
+        <v>8.386626770747089e-15</v>
       </c>
       <c r="K5">
-        <v>30</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -608,34 +608,34 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="C6">
-        <v>6.380809795566059</v>
+        <v>0.5967762292932864</v>
       </c>
       <c r="D6">
-        <v>0.1435430695320799</v>
+        <v>0.0144814315488388</v>
       </c>
       <c r="E6">
-        <v>3.265438079660177</v>
+        <v>0.3368106220879001</v>
       </c>
       <c r="F6">
-        <v>1.418164207188511e-07</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.06075071653480218</v>
+        <v>0.07670325099191222</v>
       </c>
       <c r="H6">
-        <v>0.6341438957377079</v>
+        <v>0.8158936334077829</v>
       </c>
       <c r="I6">
-        <v>2.909453587146678</v>
+        <v>3.320969459540207</v>
       </c>
       <c r="J6">
-        <v>-1.01844458792281e-14</v>
+        <v>2.122400379543156e-14</v>
       </c>
       <c r="K6">
-        <v>30</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -643,34 +643,34 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.9999999999999994</v>
       </c>
       <c r="C7">
-        <v>3.567888816915884</v>
+        <v>0.838564129162174</v>
       </c>
       <c r="D7">
-        <v>0.1433839153537295</v>
+        <v>0.01665466838797805</v>
       </c>
       <c r="E7">
-        <v>3.366916192389526</v>
+        <v>0.3817712502574175</v>
       </c>
       <c r="F7">
-        <v>4.123936309411831e-08</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.2965439946159347</v>
+        <v>0.02828557347831353</v>
       </c>
       <c r="H7">
-        <v>0.5815430501635944</v>
+        <v>0.7837045324610361</v>
       </c>
       <c r="I7">
-        <v>3.786860095324411</v>
+        <v>3.623692066263507</v>
       </c>
       <c r="J7">
-        <v>2.592520792638203e-15</v>
+        <v>1.297079016131778e-14</v>
       </c>
       <c r="K7">
-        <v>37</v>
+        <v>997</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -678,34 +678,34 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="C8">
-        <v>0.02884030168999363</v>
+        <v>0.0411574724102992</v>
       </c>
       <c r="D8">
-        <v>0.1965765756382262</v>
+        <v>0.01410740279886958</v>
       </c>
       <c r="E8">
-        <v>4.585481204082646</v>
+        <v>0.3129250543874262</v>
       </c>
       <c r="F8">
-        <v>1.673343332618078e-05</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.9950220535642406</v>
+        <v>0.8953935720716315</v>
       </c>
       <c r="H8">
-        <v>0.4549770928067196</v>
+        <v>0.8644336197950682</v>
       </c>
       <c r="I8">
-        <v>5.221496034255939</v>
+        <v>3.016645558972559</v>
       </c>
       <c r="J8">
-        <v>7.105427357601002e-15</v>
+        <v>8.670420218642236e-15</v>
       </c>
       <c r="K8">
-        <v>33</v>
+        <v>790</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -713,34 +713,34 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1.000000000000002</v>
       </c>
       <c r="C9">
-        <v>5.086357067735555</v>
+        <v>0.2688994068953255</v>
       </c>
       <c r="D9">
-        <v>0.06930718222530308</v>
+        <v>0.01770665261890524</v>
       </c>
       <c r="E9">
-        <v>1.480981933674747</v>
+        <v>0.3957801906792482</v>
       </c>
       <c r="F9">
-        <v>9.108925829895073e-15</v>
+        <v>1.578938943504622e-317</v>
       </c>
       <c r="G9">
-        <v>0.0018102221604539</v>
+        <v>0.497027091671329</v>
       </c>
       <c r="H9">
-        <v>0.8777311088258974</v>
+        <v>0.7560763277210524</v>
       </c>
       <c r="I9">
-        <v>1.723169989892944</v>
+        <v>4.385327212346684</v>
       </c>
       <c r="J9">
-        <v>-1.260640337638887e-14</v>
+        <v>-1.350789293976524e-15</v>
       </c>
       <c r="K9">
-        <v>31</v>
+        <v>1031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>